<commit_message>
Fixed comments and removed isAuthenticated where not necessary
</commit_message>
<xml_diff>
--- a/Supporting Content/Uni Hub Test Cases.xlsx
+++ b/Supporting Content/Uni Hub Test Cases.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="614" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E2D5131-24F6-459A-9424-65DACC5D7A44}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Documents/uni-hub/Supporting Content/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899B2F7E-5C51-A74F-B106-23295AD22AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="36000" windowHeight="22620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -180,9 +185,6 @@
     <t>Profile badges correctly update depending on a user's post count, comment count, community count, achievement count, follower count, and following count.</t>
   </si>
   <si>
-    <t>50 posts, comments, communitites joined, achievements posted, followers, following. Monitor the profile badges at each number, particularly 25 and 50.</t>
-  </si>
-  <si>
     <t>Profile badges update as expected.</t>
   </si>
   <si>
@@ -442,13 +444,16 @@
   </si>
   <si>
     <t>Only the community leader can pin and re-order posts.</t>
+  </si>
+  <si>
+    <t>5, 5-15 and 15+ posts, comments, communitites joined, achievements posted, followers, following. Monitor the profile badges at each number, particularly 5 and 15.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +552,16 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -568,16 +583,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -592,16 +597,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3CB2074-EE70-486C-B34F-AA94A31A0962}" name="Table1" displayName="Table1" ref="A1:E45" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3CB2074-EE70-486C-B34F-AA94A31A0962}" name="Table1" displayName="Table1" ref="A1:E45" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:E45" xr:uid="{E3CB2074-EE70-486C-B34F-AA94A31A0962}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{27EE3CE2-755F-4CA0-A4BE-43F61A5B0992}" name="Test Case ID" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{27EE3CE2-755F-4CA0-A4BE-43F61A5B0992}" name="Test Case ID" dataDxfId="5">
       <calculatedColumnFormula>ROW(A2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E072D760-CDAB-453B-BDB7-C5CA27DF6144}" name="Test Description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{08698D23-1360-4A54-83F4-F300212DDAA3}" name="Test Steps" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{F7127C63-23D3-43B0-B24E-D5D96D742A44}" name="Expected Result" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{9C9E73C2-8F0B-44DD-9538-572F2C73BE24}" name="Pass/Fail" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E072D760-CDAB-453B-BDB7-C5CA27DF6144}" name="Test Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{08698D23-1360-4A54-83F4-F300212DDAA3}" name="Test Steps" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F7127C63-23D3-43B0-B24E-D5D96D742A44}" name="Expected Result" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{9C9E73C2-8F0B-44DD-9538-572F2C73BE24}" name="Pass/Fail" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -926,20 +931,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" customHeight="1">
+    <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -956,7 +961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="189" customHeight="1">
+    <row r="2" spans="1:5" ht="189" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <f t="shared" ref="A2:A31" si="0">ROW(A2)-1</f>
         <v>1</v>
@@ -974,7 +979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="153" customHeight="1">
+    <row r="3" spans="1:5" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -992,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="130.5" customHeight="1">
+    <row r="4" spans="1:5" ht="130.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1010,7 +1015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="245.25" customHeight="1">
+    <row r="5" spans="1:5" ht="245.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1028,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="259.5" customHeight="1">
+    <row r="6" spans="1:5" ht="259.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1046,7 +1051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="94.5" customHeight="1">
+    <row r="7" spans="1:5" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1064,7 +1069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="109.5" customHeight="1">
+    <row r="8" spans="1:5" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1082,7 +1087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="159.75" customHeight="1">
+    <row r="9" spans="1:5" ht="159.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1100,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="115.5" customHeight="1">
+    <row r="10" spans="1:5" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1118,7 +1123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="185.25" customHeight="1">
+    <row r="11" spans="1:5" ht="185.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1136,7 +1141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="162.75" customHeight="1">
+    <row r="12" spans="1:5" ht="162.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1154,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="91.5" customHeight="1">
+    <row r="13" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1172,7 +1177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="106.5" customHeight="1">
+    <row r="14" spans="1:5" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1190,7 +1195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="72.75" customHeight="1">
+    <row r="15" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1208,7 +1213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="111" customHeight="1">
+    <row r="16" spans="1:5" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1217,532 +1222,532 @@
         <v>48</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="160.5" customHeight="1">
-      <c r="A17" s="8">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="177" customHeight="1">
-      <c r="A18" s="8">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="192" customHeight="1">
-      <c r="A19" s="8">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="151.5" customHeight="1">
-      <c r="A20" s="8">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="160.5" customHeight="1">
-      <c r="A21" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="138.75" customHeight="1">
-      <c r="A22" s="8">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="161.25" customHeight="1">
-      <c r="A23" s="8">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="72" customHeight="1">
-      <c r="A24" s="8">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="153" customHeight="1">
-      <c r="A25" s="8">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="114" customHeight="1">
-      <c r="A26" s="8">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="240" customHeight="1">
-      <c r="A27" s="8">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="87" customHeight="1">
-      <c r="A28" s="8">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="60" customHeight="1">
-      <c r="A29" s="8">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="81.75" customHeight="1">
-      <c r="A30" s="8">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="111" customHeight="1">
-      <c r="A31" s="8">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="E31" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="52.5" customHeight="1">
+    <row r="32" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <f t="shared" ref="A32:A45" si="1">ROW(A32)-1</f>
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="E32" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="93" customHeight="1">
+    <row r="33" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="D33" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="E33" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="58.5" customHeight="1">
+    <row r="34" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="D34" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="E34" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="126" customHeight="1">
+    <row r="35" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="E35" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="63.75" customHeight="1">
+    <row r="36" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="E36" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="102" customHeight="1">
+    <row r="37" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="E37" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="97.5" customHeight="1">
+    <row r="38" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="E38" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="94.5" customHeight="1">
+    <row r="39" spans="1:5" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="E39" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="100.5" customHeight="1">
+    <row r="40" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="E40" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="150" customHeight="1">
+    <row r="41" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="E41" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="93" customHeight="1">
+    <row r="42" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="E42" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="52.5" customHeight="1">
+    <row r="43" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="E43" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="52.5" customHeight="1">
+    <row r="44" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>133</v>
-      </c>
       <c r="E44" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="112.5" customHeight="1">
+    <row r="45" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>8</v>
@@ -1750,7 +1755,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>